<commit_message>
For submission to journal
</commit_message>
<xml_diff>
--- a/Example_p_LDA_calculation.xlsx
+++ b/Example_p_LDA_calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivanna\Documents\DATA\Ivanna\Research_Book\SCI_Parameter_Combination\code_eNeuro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivanna\Documents\DATA\Ivanna\Research_Book\SCI_Parameter_Combination\code_GaitParamCombSCI_GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>